<commit_message>
fixed k-fold split mistake
</commit_message>
<xml_diff>
--- a/model_comparison.xlsx
+++ b/model_comparison.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreawickman/saving_lives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36939E5-D1E5-704A-9C99-BAF330E29245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A314EF-DB17-1A4B-9989-24272298B96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28240" windowHeight="16340" activeTab="1" xr2:uid="{C53D87BE-9659-C740-A74D-1D1C5795C2F5}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28240" windowHeight="16340" activeTab="3" xr2:uid="{C53D87BE-9659-C740-A74D-1D1C5795C2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="binary" sheetId="3" r:id="rId1"/>
     <sheet name="multiclass" sheetId="1" r:id="rId2"/>
     <sheet name="prediction" sheetId="2" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="146">
   <si>
     <t>genome_lrtt</t>
   </si>
@@ -358,9 +359,6 @@
     <t>** for set knots</t>
   </si>
   <si>
-    <t>** for adaptive knots</t>
-  </si>
-  <si>
     <t>Tanya_sqrt</t>
   </si>
   <si>
@@ -422,18 +420,76 @@
   </si>
   <si>
     <t xml:space="preserve">True positive Rate  </t>
+  </si>
+  <si>
+    <t>THRESHOLD:  12 MONTHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROC AUC: </t>
+  </si>
+  <si>
+    <t>Precision (Non Recent)</t>
+  </si>
+  <si>
+    <t>Precision (Recent)</t>
+  </si>
+  <si>
+    <t>Recall (Non Recent)</t>
+  </si>
+  <si>
+    <t>Recall (Recent)</t>
+  </si>
+  <si>
+    <t>F1 Score (Non Recent)</t>
+  </si>
+  <si>
+    <t>F1 Score (Recent)</t>
+  </si>
+  <si>
+    <t>Average Precision</t>
+  </si>
+  <si>
+    <t>Training Time</t>
+  </si>
+  <si>
+    <t>Smoothed?</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>LOOCV MEAN ACC:</t>
+  </si>
+  <si>
+    <t>RFECV1</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>B*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*BEST FORMING FOR BSPLINE SMOOTHED </t>
+  </si>
+  <si>
+    <t>lrtt_coeff_0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,8 +605,28 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +679,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFED9DA1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0E6F5"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -664,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -784,7 +866,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -805,6 +886,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -820,706 +924,45 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <border>
         <left style="thin">
@@ -1636,6 +1079,56 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1982,83 +1475,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15294C40-2ADD-B846-8AE6-90A6FCEAB524}">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="11.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="22">
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:20" ht="22">
+      <c r="C1" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:15" ht="19">
-      <c r="A2" s="67" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+    </row>
+    <row r="2" spans="1:20" s="27" customFormat="1" ht="19">
+      <c r="A2" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="81" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="76"/>
+      <c r="G2" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+    </row>
+    <row r="3" spans="1:20" ht="18">
+      <c r="A3" s="75"/>
+      <c r="B3" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="68"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-    </row>
-    <row r="3" spans="1:15" ht="18">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
       <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:15" s="6" customFormat="1" ht="18">
+    <row r="4" spans="1:20" s="6" customFormat="1" ht="18">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>43</v>
+      <c r="B4" s="29">
+        <v>0.51</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -2068,21 +1584,31 @@
         <v>26</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" s="6" customFormat="1" ht="18">
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" s="6" customFormat="1" ht="18">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>44</v>
+      <c r="B5" s="29">
+        <v>0.22</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>26</v>
@@ -2092,21 +1618,31 @@
         <v>26</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" s="6" customFormat="1" ht="18">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" s="6" customFormat="1" ht="18">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>45</v>
+      <c r="B6" s="29">
+        <v>0.24</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>26</v>
@@ -2116,21 +1652,31 @@
         <v>26</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" s="6" customFormat="1" ht="18">
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" s="6" customFormat="1" ht="18">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>55</v>
+      <c r="B7" s="29">
+        <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>26</v>
@@ -2139,20 +1685,29 @@
         <v>26</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" s="6" customFormat="1" ht="18">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" s="6" customFormat="1" ht="18">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>81</v>
+      <c r="B8" s="29">
+        <v>0.19</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>26</v>
@@ -2162,21 +1717,29 @@
         <v>26</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" s="6" customFormat="1" ht="18">
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" s="6" customFormat="1" ht="18">
       <c r="A9" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>55</v>
+      <c r="B9" s="29">
+        <v>0</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2184,19 +1747,25 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" s="6" customFormat="1" ht="18">
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" s="6" customFormat="1" ht="18">
       <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>88</v>
+      <c r="B10" s="29">
+        <v>0.05</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2204,14 +1773,20 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="1:20">
       <c r="B11" s="30"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -2220,12 +1795,12 @@
       <c r="K11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" s="9" customFormat="1" ht="18">
+    <row r="12" spans="1:20" s="9" customFormat="1" ht="18">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>43</v>
+      <c r="B12" s="31">
+        <v>0.51</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>26</v>
@@ -2239,21 +1814,27 @@
       <c r="F12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="G12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:15" s="9" customFormat="1" ht="18">
+    <row r="13" spans="1:20" s="9" customFormat="1" ht="18">
       <c r="A13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>56</v>
+      <c r="B13" s="31">
+        <v>0.11</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>26</v>
@@ -2261,14 +1842,17 @@
       <c r="E13" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="G13" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:15" s="9" customFormat="1" ht="18">
+    <row r="14" spans="1:20" s="9" customFormat="1" ht="18">
       <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>47</v>
+      <c r="B14" s="31">
+        <v>0.23</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>26</v>
@@ -2282,21 +1866,27 @@
       <c r="F14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="G14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:15" s="9" customFormat="1" ht="18">
+    <row r="15" spans="1:20" s="9" customFormat="1" ht="18">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>83</v>
+      <c r="B15" s="31">
+        <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>26</v>
@@ -2308,18 +1898,24 @@
         <v>26</v>
       </c>
       <c r="F15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:15" s="9" customFormat="1" ht="18">
+    <row r="16" spans="1:20" s="9" customFormat="1" ht="18">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>57</v>
+      <c r="B16" s="31">
+        <v>0.09</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>26</v>
@@ -2329,14 +1925,17 @@
         <v>26</v>
       </c>
       <c r="F16" s="8"/>
+      <c r="G16" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="N16" s="8"/>
     </row>
     <row r="17" spans="1:14" s="9" customFormat="1" ht="18">
       <c r="A17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>55</v>
+      <c r="B17" s="31">
+        <v>0</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2348,8 +1947,8 @@
       <c r="A18" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>85</v>
+      <c r="B18" s="31">
+        <v>0.04</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2360,7 +1959,6 @@
     <row r="19" spans="1:14">
       <c r="B19" s="30"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2369,8 +1967,8 @@
       <c r="A20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>50</v>
+      <c r="B20" s="32">
+        <v>0.44</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>26</v>
@@ -2384,9 +1982,15 @@
       <c r="F20" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="G20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -2397,8 +2001,8 @@
       <c r="A21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="32" t="s">
-        <v>57</v>
+      <c r="B21" s="32">
+        <v>0.09</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>26</v>
@@ -2406,8 +2010,9 @@
       <c r="E21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="G21" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -2417,8 +2022,8 @@
       <c r="A22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>58</v>
+      <c r="B22" s="32">
+        <v>0.13</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>26</v>
@@ -2426,8 +2031,9 @@
       <c r="E22" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="G22" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -2437,13 +2043,12 @@
       <c r="A23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="32" t="s">
-        <v>82</v>
+      <c r="B23" s="32">
+        <v>0.02</v>
       </c>
       <c r="C23" s="11"/>
       <c r="E23" s="11"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -2453,13 +2058,16 @@
       <c r="A24" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="32" t="s">
-        <v>89</v>
+      <c r="B24" s="32">
+        <v>0.08</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>26</v>
       </c>
       <c r="N24" s="11"/>
@@ -2468,8 +2076,8 @@
       <c r="A25" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>55</v>
+      <c r="B25" s="32">
+        <v>0</v>
       </c>
       <c r="C25" s="11"/>
       <c r="E25" s="11"/>
@@ -2479,8 +2087,8 @@
       <c r="A26" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>86</v>
+      <c r="B26" s="32">
+        <v>0.03</v>
       </c>
       <c r="C26" s="11"/>
       <c r="E26" s="11"/>
@@ -2493,8 +2101,8 @@
       <c r="A28" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="33" t="s">
-        <v>48</v>
+      <c r="B28" s="33">
+        <v>0.31</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>26</v>
@@ -2508,9 +2116,15 @@
       <c r="F28" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
+      <c r="G28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
@@ -2521,8 +2135,8 @@
       <c r="A29" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="33" t="s">
-        <v>49</v>
+      <c r="B29" s="33">
+        <v>0.25</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>26</v>
@@ -2530,9 +2144,12 @@
       <c r="E29" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
       <c r="N29" s="14"/>
@@ -2541,13 +2158,16 @@
       <c r="A30" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="33" t="s">
-        <v>59</v>
+      <c r="B30" s="33">
+        <v>0.2</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>26</v>
       </c>
       <c r="J30" s="14"/>
@@ -2557,8 +2177,8 @@
       <c r="A31" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="33" t="s">
-        <v>55</v>
+      <c r="B31" s="33">
+        <v>0</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>26</v>
@@ -2570,6 +2190,12 @@
         <v>26</v>
       </c>
       <c r="F31" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>26</v>
       </c>
       <c r="L31" s="14"/>
@@ -2580,8 +2206,8 @@
       <c r="A32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="33" t="s">
-        <v>52</v>
+      <c r="B32" s="33">
+        <v>0.21</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>26</v>
@@ -2589,9 +2215,12 @@
       <c r="E32" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
+      <c r="G32" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
     </row>
@@ -2599,11 +2228,10 @@
       <c r="A33" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="33" t="s">
-        <v>84</v>
+      <c r="B33" s="33">
+        <v>0.01</v>
       </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
@@ -2612,11 +2240,10 @@
       <c r="A34" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>87</v>
+      <c r="B34" s="33">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
@@ -2636,8 +2263,8 @@
       <c r="A37" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="34" t="s">
-        <v>60</v>
+      <c r="B37" s="34">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>26</v>
@@ -2649,6 +2276,12 @@
         <v>26</v>
       </c>
       <c r="F37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="18" t="s">
         <v>26</v>
       </c>
       <c r="L37" s="18"/>
@@ -2659,8 +2292,8 @@
       <c r="A38" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="34" t="s">
-        <v>45</v>
+      <c r="B38" s="34">
+        <v>0.24</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>26</v>
@@ -2674,9 +2307,15 @@
       <c r="F38" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="G38" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
       <c r="L38" s="18"/>
@@ -2696,6 +2335,9 @@
       <c r="F39" s="18" t="s">
         <v>26</v>
       </c>
+      <c r="H39" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
     </row>
@@ -2703,13 +2345,16 @@
       <c r="A40" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="34" t="s">
-        <v>56</v>
+      <c r="B40" s="34">
+        <v>0.11</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2736,15 +2381,17 @@
       <c r="A44" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="35" t="s">
-        <v>61</v>
+      <c r="B44" s="35">
+        <v>0.41</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
+      <c r="I44" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="J44" s="21"/>
       <c r="K44" s="21"/>
     </row>
@@ -2757,13 +2404,15 @@
       <c r="A46" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="35" t="s">
-        <v>62</v>
+      <c r="B46" s="35">
+        <v>0.28000000000000003</v>
       </c>
       <c r="E46" s="21"/>
       <c r="F46" s="21"/>
       <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
+      <c r="I46" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="J46" s="21"/>
       <c r="K46" s="21"/>
     </row>
@@ -2771,8 +2420,8 @@
       <c r="A47" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="35" t="s">
-        <v>47</v>
+      <c r="B47" s="35">
+        <v>0.23</v>
       </c>
     </row>
     <row r="48" spans="1:14" s="20" customFormat="1">
@@ -2815,11 +2464,13 @@
       <c r="A54" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="35" t="s">
-        <v>63</v>
+      <c r="B54" s="35">
+        <v>0.26</v>
       </c>
       <c r="F54" s="21"/>
-      <c r="I54" s="21"/>
+      <c r="I54" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="55" spans="1:19" ht="18">
       <c r="A55" s="24" t="s">
@@ -2844,61 +2495,67 @@
       <c r="R55" s="24"/>
       <c r="S55" s="24"/>
     </row>
-    <row r="56" spans="1:19" s="23" customFormat="1" ht="18">
-      <c r="A56" s="22" t="s">
+    <row r="56" spans="1:19" s="87" customFormat="1" ht="18">
+      <c r="A56" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="26">
+      <c r="B56" s="83"/>
+      <c r="C56" s="84">
         <v>0.83225806451612905</v>
       </c>
-      <c r="D56" s="26">
+      <c r="D56" s="84">
         <v>0.825806451612903</v>
       </c>
-      <c r="E56" s="36">
+      <c r="E56" s="85">
         <v>0.84</v>
       </c>
-      <c r="F56" s="36">
+      <c r="F56" s="85">
         <v>0.825806451612903</v>
       </c>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
-      <c r="L56" s="25"/>
-      <c r="M56" s="26"/>
-      <c r="N56" s="25"/>
-      <c r="O56" s="25"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="25"/>
-      <c r="R56" s="25"/>
-      <c r="S56" s="25"/>
-    </row>
-    <row r="57" spans="1:19" s="23" customFormat="1" ht="18">
-      <c r="A57" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" s="22"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25">
+      <c r="G56" s="85">
+        <v>0.76129999999999998</v>
+      </c>
+      <c r="H56" s="85">
+        <v>0.75480000000000003</v>
+      </c>
+      <c r="I56" s="85">
+        <v>0.78064500000000003</v>
+      </c>
+      <c r="J56" s="85"/>
+      <c r="K56" s="85"/>
+      <c r="L56" s="86"/>
+      <c r="M56" s="84"/>
+      <c r="N56" s="86"/>
+      <c r="O56" s="86"/>
+      <c r="P56" s="86"/>
+      <c r="Q56" s="86"/>
+      <c r="R56" s="86"/>
+      <c r="S56" s="86"/>
+    </row>
+    <row r="57" spans="1:19" s="87" customFormat="1" ht="18">
+      <c r="A57" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" s="83"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="86"/>
+      <c r="E57" s="86">
         <v>0.82469999999999999</v>
       </c>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
-      <c r="L57" s="25"/>
-      <c r="M57" s="25"/>
-      <c r="N57" s="25"/>
-      <c r="O57" s="25"/>
-      <c r="P57" s="25"/>
-      <c r="Q57" s="25"/>
-      <c r="R57" s="25"/>
-      <c r="S57" s="25"/>
+      <c r="F57" s="86"/>
+      <c r="G57" s="86"/>
+      <c r="H57" s="86"/>
+      <c r="I57" s="86"/>
+      <c r="J57" s="86"/>
+      <c r="K57" s="86"/>
+      <c r="L57" s="86"/>
+      <c r="M57" s="86"/>
+      <c r="N57" s="86"/>
+      <c r="O57" s="86"/>
+      <c r="P57" s="86"/>
+      <c r="Q57" s="86"/>
+      <c r="R57" s="86"/>
+      <c r="S57" s="86"/>
     </row>
     <row r="58" spans="1:19" ht="18">
       <c r="A58" s="24"/>
@@ -2923,16 +2580,22 @@
     </row>
     <row r="59" spans="1:19" ht="18">
       <c r="A59" s="24" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
       <c r="E59" s="24"/>
       <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
+      <c r="G59" s="88">
+        <v>0.85060000000000002</v>
+      </c>
+      <c r="H59" s="88">
+        <v>0.84870000000000001</v>
+      </c>
+      <c r="I59" s="88">
+        <v>0.84379199999999999</v>
+      </c>
       <c r="J59" s="24"/>
       <c r="K59" s="24"/>
       <c r="L59" s="24"/>
@@ -2944,70 +2607,211 @@
       <c r="R59" s="24"/>
       <c r="S59" s="24"/>
     </row>
-    <row r="60" spans="1:19" s="23" customFormat="1" ht="18">
-      <c r="A60" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="36">
-        <v>0.85</v>
-      </c>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="36"/>
-      <c r="J60" s="36"/>
-      <c r="K60" s="36"/>
-      <c r="L60" s="25"/>
-      <c r="M60" s="26"/>
-      <c r="N60" s="25"/>
-      <c r="O60" s="25"/>
-      <c r="P60" s="25"/>
-      <c r="Q60" s="25"/>
-      <c r="R60" s="25"/>
-      <c r="S60" s="25"/>
-    </row>
-    <row r="61" spans="1:19" s="23" customFormat="1" ht="18">
-      <c r="A61" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="25"/>
-      <c r="J61" s="25"/>
-      <c r="K61" s="25"/>
-      <c r="L61" s="25"/>
-      <c r="M61" s="25"/>
-      <c r="N61" s="25"/>
-      <c r="O61" s="25"/>
-      <c r="P61" s="25"/>
-      <c r="Q61" s="25"/>
-      <c r="R61" s="25"/>
-      <c r="S61" s="25"/>
+    <row r="60" spans="1:19" ht="18">
+      <c r="A60" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="88">
+        <v>0.7419</v>
+      </c>
+      <c r="H60" s="88">
+        <v>0.73019999999999996</v>
+      </c>
+      <c r="I60" s="88">
+        <v>0.77049199999999995</v>
+      </c>
+      <c r="J60" s="24"/>
+      <c r="K60" s="24"/>
+      <c r="L60" s="24"/>
+      <c r="M60" s="24"/>
+      <c r="N60" s="24"/>
+      <c r="O60" s="24"/>
+      <c r="P60" s="24"/>
+      <c r="Q60" s="24"/>
+      <c r="R60" s="24"/>
+      <c r="S60" s="24"/>
+    </row>
+    <row r="61" spans="1:19" ht="18">
+      <c r="A61" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="88">
+        <v>0.7742</v>
+      </c>
+      <c r="H61" s="88">
+        <v>0.77170000000000005</v>
+      </c>
+      <c r="I61" s="88">
+        <v>0.78723399999999999</v>
+      </c>
+      <c r="J61" s="24"/>
+      <c r="K61" s="24"/>
+      <c r="L61" s="24"/>
+      <c r="M61" s="24"/>
+      <c r="N61" s="24"/>
+      <c r="O61" s="24"/>
+      <c r="P61" s="24"/>
+      <c r="Q61" s="24"/>
+      <c r="R61" s="24"/>
+      <c r="S61" s="24"/>
+    </row>
+    <row r="62" spans="1:19" ht="18">
+      <c r="A62" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="88">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="H62" s="88">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="I62" s="88">
+        <v>0.86834900000000004</v>
+      </c>
+      <c r="J62" s="24"/>
+      <c r="K62" s="24"/>
+      <c r="L62" s="24"/>
+      <c r="M62" s="24"/>
+      <c r="N62" s="24"/>
+      <c r="O62" s="24"/>
+      <c r="P62" s="24"/>
+      <c r="Q62" s="24"/>
+      <c r="R62" s="24"/>
+      <c r="S62" s="24"/>
+    </row>
+    <row r="63" spans="1:19" ht="18">
+      <c r="A63" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="88">
+        <v>0.68659999999999999</v>
+      </c>
+      <c r="H63" s="88">
+        <v>0.68659999999999999</v>
+      </c>
+      <c r="I63" s="88">
+        <v>0.70149300000000003</v>
+      </c>
+      <c r="J63" s="24"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="24"/>
+      <c r="N63" s="24"/>
+      <c r="O63" s="24"/>
+      <c r="P63" s="24"/>
+      <c r="Q63" s="24"/>
+      <c r="R63" s="24"/>
+      <c r="S63" s="24"/>
+    </row>
+    <row r="64" spans="1:19" ht="18">
+      <c r="A64" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="88">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="H64" s="88">
+        <v>0.80679999999999996</v>
+      </c>
+      <c r="I64" s="88">
+        <v>0.84090900000000002</v>
+      </c>
+      <c r="J64" s="24"/>
+      <c r="K64" s="24"/>
+      <c r="L64" s="24"/>
+      <c r="M64" s="24"/>
+      <c r="N64" s="24"/>
+      <c r="O64" s="24"/>
+      <c r="P64" s="24"/>
+      <c r="Q64" s="24"/>
+      <c r="R64" s="24"/>
+      <c r="S64" s="24"/>
+    </row>
+    <row r="65" spans="1:10" ht="18">
+      <c r="A65" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G65" s="88">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="H65" s="88">
+        <v>0.7077</v>
+      </c>
+      <c r="I65" s="88">
+        <v>0.734375</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="18">
+      <c r="A66" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G66" s="88">
+        <v>0.79559999999999997</v>
+      </c>
+      <c r="H66" s="88">
+        <v>0.78890000000000005</v>
+      </c>
+      <c r="I66" s="88">
+        <v>0.81318699999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="18">
+      <c r="A68" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="G68" s="89">
+        <v>188.109129</v>
+      </c>
+      <c r="H68" s="90"/>
+      <c r="I68" s="91">
+        <v>140.73164</v>
+      </c>
+      <c r="J68" s="90"/>
+    </row>
+    <row r="74" spans="1:10" ht="19">
+      <c r="A74" s="82" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C56:H56 L56:O56">
-    <cfRule type="top10" dxfId="50" priority="2" stopIfTrue="1" rank="1"/>
+  <conditionalFormatting sqref="A59:XFD59">
+    <cfRule type="top10" dxfId="9" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60:H60 L60:O60">
-    <cfRule type="top10" dxfId="49" priority="1" stopIfTrue="1" rank="1"/>
+  <conditionalFormatting sqref="A56:XFD56">
+    <cfRule type="top10" dxfId="8" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3017,8 +2821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE8C9DF-FF8E-364F-96CD-2337D270FDFA}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3031,32 +2835,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" thickBot="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68" t="s">
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="68"/>
+      <c r="N1" s="76"/>
     </row>
     <row r="2" spans="1:15" ht="18">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
       <c r="C2" s="3" t="s">
         <v>64</v>
       </c>
@@ -4249,7 +4053,7 @@
     </row>
     <row r="58" spans="1:19" ht="18">
       <c r="A58" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B58" s="24"/>
       <c r="C58" s="24"/>
@@ -4272,7 +4076,7 @@
     </row>
     <row r="59" spans="1:19" ht="18">
       <c r="A59" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
@@ -4295,17 +4099,17 @@
     </row>
     <row r="60" spans="1:19" ht="18">
       <c r="A60" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:19" ht="18">
       <c r="A63" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="18">
       <c r="A64" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -4317,7 +4121,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C55:H55 L55:O55">
-    <cfRule type="top10" dxfId="48" priority="1" stopIfTrue="1" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="1" stopIfTrue="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4327,8 +4131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEEB0B7-53EA-2E45-8661-88EAB58A8768}">
   <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView topLeftCell="M45" zoomScale="136" workbookViewId="0">
-      <selection activeCell="S51" sqref="S51"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B52" sqref="A1:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4356,10 +4160,10 @@
         <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>98</v>
@@ -4368,43 +4172,43 @@
         <v>103</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="O1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="6" customFormat="1" ht="18">
@@ -5978,273 +5782,273 @@
     </row>
     <row r="53" spans="1:20" ht="18">
       <c r="A53" s="1"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
-      <c r="H53" s="64"/>
-      <c r="J53" s="64"/>
-    </row>
-    <row r="54" spans="1:20" s="60" customFormat="1" ht="18">
-      <c r="A54" s="70" t="s">
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="H53" s="63"/>
+      <c r="J53" s="63"/>
+    </row>
+    <row r="54" spans="1:20" s="59" customFormat="1" ht="18">
+      <c r="A54" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="70"/>
-      <c r="C54" s="62">
+      <c r="B54" s="78"/>
+      <c r="C54" s="61">
         <v>0.586269697384737</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="61">
         <v>0.60088966138840505</v>
       </c>
-      <c r="E54" s="62">
+      <c r="E54" s="61">
         <v>0.63046306311287903</v>
       </c>
-      <c r="F54" s="59"/>
-      <c r="G54" s="62">
+      <c r="F54" s="58"/>
+      <c r="G54" s="61">
         <v>0.62576749573437596</v>
       </c>
-      <c r="H54" s="62">
+      <c r="H54" s="61">
         <v>0.60928413931048897</v>
       </c>
-      <c r="I54" s="62">
+      <c r="I54" s="61">
         <v>0.59887012524755701</v>
       </c>
-      <c r="J54" s="62">
+      <c r="J54" s="61">
         <v>0.60887218522029296</v>
       </c>
-      <c r="K54" s="62">
+      <c r="K54" s="61">
         <v>0.61981180200570196</v>
       </c>
-      <c r="L54" s="62">
+      <c r="L54" s="61">
         <v>0.62331113905808899</v>
       </c>
-      <c r="M54" s="62">
+      <c r="M54" s="61">
         <v>0.619816234503201</v>
       </c>
-      <c r="N54" s="62">
+      <c r="N54" s="61">
         <v>0.63606239035258205</v>
       </c>
-      <c r="O54" s="62">
+      <c r="O54" s="61">
         <v>0.63164212242349504</v>
       </c>
-      <c r="P54" s="62">
+      <c r="P54" s="61">
         <v>0.62967240006881997</v>
       </c>
-      <c r="Q54" s="59"/>
-      <c r="R54" s="62">
+      <c r="Q54" s="58"/>
+      <c r="R54" s="61">
         <v>0.63451653110765505</v>
       </c>
-      <c r="S54" s="62">
+      <c r="S54" s="61">
         <v>0.64471358543291102</v>
       </c>
-      <c r="T54" s="59"/>
-    </row>
-    <row r="55" spans="1:20" s="60" customFormat="1" ht="18">
-      <c r="A55" s="70" t="s">
+      <c r="T54" s="58"/>
+    </row>
+    <row r="55" spans="1:20" s="59" customFormat="1" ht="18">
+      <c r="A55" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="70"/>
-      <c r="C55" s="62"/>
-      <c r="D55" s="62">
+      <c r="B55" s="78"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61">
         <v>0.610357441756053</v>
       </c>
-      <c r="E55" s="62">
+      <c r="E55" s="61">
         <v>0.61576164145006596</v>
       </c>
-      <c r="F55" s="62">
+      <c r="F55" s="61">
         <v>0.60792363051465803</v>
       </c>
-      <c r="G55" s="62"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="62"/>
-      <c r="J55" s="62"/>
-      <c r="K55" s="62"/>
-      <c r="L55" s="62">
+      <c r="G55" s="61"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="61"/>
+      <c r="J55" s="61"/>
+      <c r="K55" s="61"/>
+      <c r="L55" s="61">
         <v>0.62109808579383297</v>
       </c>
-      <c r="M55" s="62"/>
-      <c r="N55" s="62">
+      <c r="M55" s="61"/>
+      <c r="N55" s="61">
         <v>0.62273936370390004</v>
       </c>
-      <c r="O55" s="62">
+      <c r="O55" s="61">
         <v>0.62284574248222402</v>
       </c>
-      <c r="P55" s="62">
+      <c r="P55" s="61">
         <v>0.62637656308414802</v>
       </c>
-      <c r="Q55" s="72">
+      <c r="Q55" s="67">
         <v>0.61887347172287199</v>
       </c>
-      <c r="R55" s="62">
-        <v>0.62862330802919897</v>
-      </c>
-      <c r="S55" s="62">
+      <c r="R55" s="61">
+        <v>0.63153311427661496</v>
+      </c>
+      <c r="S55" s="61">
         <v>0.62651988994835595</v>
       </c>
-      <c r="T55" s="59"/>
-    </row>
-    <row r="56" spans="1:20" s="80" customFormat="1" ht="18">
-      <c r="A56" s="75" t="s">
+      <c r="T55" s="58"/>
+    </row>
+    <row r="56" spans="1:20" s="23" customFormat="1" ht="18">
+      <c r="A56" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="75"/>
-      <c r="C56" s="76">
+      <c r="B56" s="77"/>
+      <c r="C56" s="26">
         <v>0.29971413609342501</v>
       </c>
-      <c r="D56" s="76">
+      <c r="D56" s="26">
         <v>0.28912315483491402</v>
       </c>
-      <c r="E56" s="76">
+      <c r="E56" s="26">
         <v>0.176309290904334</v>
       </c>
-      <c r="F56" s="76"/>
-      <c r="G56" s="77">
+      <c r="F56" s="26"/>
+      <c r="G56" s="36">
         <v>0.17854958699454701</v>
       </c>
-      <c r="H56" s="76">
+      <c r="H56" s="26">
         <v>0.18641393989875099</v>
       </c>
-      <c r="I56" s="77">
+      <c r="I56" s="36">
         <v>0.19138255670434001</v>
       </c>
-      <c r="J56" s="77">
+      <c r="J56" s="36">
         <v>0.18661048678291201</v>
       </c>
-      <c r="K56" s="77">
+      <c r="K56" s="36">
         <v>0.18139110034092801</v>
       </c>
-      <c r="L56" s="76">
+      <c r="L56" s="26">
         <v>0.17972153615733499</v>
       </c>
-      <c r="M56" s="77">
+      <c r="M56" s="36">
         <v>0.181388985557769</v>
       </c>
-      <c r="N56" s="76">
+      <c r="N56" s="26">
         <v>0.173637803113453</v>
       </c>
-      <c r="O56" s="76">
+      <c r="O56" s="26">
         <v>0.17574675143875301</v>
       </c>
-      <c r="P56" s="76">
+      <c r="P56" s="26">
         <v>0.17668652312857799</v>
       </c>
-      <c r="Q56" s="78"/>
-      <c r="R56" s="76">
+      <c r="Q56" s="68"/>
+      <c r="R56" s="26">
         <v>0.174375346022173</v>
       </c>
-      <c r="S56" s="76">
+      <c r="S56" s="26">
         <v>0.169510242596942</v>
       </c>
-      <c r="T56" s="79"/>
-    </row>
-    <row r="57" spans="1:20" s="80" customFormat="1" ht="18">
-      <c r="A57" s="75" t="s">
+      <c r="T56" s="25"/>
+    </row>
+    <row r="57" spans="1:20" s="23" customFormat="1" ht="18">
+      <c r="A57" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="75"/>
-      <c r="C57" s="76">
+      <c r="B57" s="77"/>
+      <c r="C57" s="26">
         <v>0.39558775936502699</v>
       </c>
-      <c r="D57" s="76">
+      <c r="D57" s="26">
         <v>0.39499289673048699</v>
       </c>
-      <c r="E57" s="76"/>
-      <c r="F57" s="79"/>
-      <c r="G57" s="76">
+      <c r="E57" s="26"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="26">
         <v>0.30997845535217899</v>
       </c>
-      <c r="H57" s="76">
+      <c r="H57" s="26">
         <v>0.31428366744859798</v>
       </c>
-      <c r="I57" s="76">
+      <c r="I57" s="26">
         <v>0.32093119588938501</v>
       </c>
-      <c r="J57" s="76">
+      <c r="J57" s="26">
         <v>0.31986127695995697</v>
       </c>
-      <c r="K57" s="76">
+      <c r="K57" s="26">
         <v>0.31242930458972701</v>
       </c>
-      <c r="L57" s="76">
+      <c r="L57" s="26">
         <v>0.31343390575387903</v>
       </c>
-      <c r="M57" s="76">
+      <c r="M57" s="26">
         <v>0.31638137524539101</v>
       </c>
-      <c r="N57" s="76">
+      <c r="N57" s="26">
         <v>0.30591222896543901</v>
       </c>
-      <c r="O57" s="76">
+      <c r="O57" s="26">
         <v>0.30572641261568101</v>
       </c>
-      <c r="P57" s="76">
+      <c r="P57" s="26">
         <v>0.30990381510897602</v>
       </c>
-      <c r="Q57" s="78"/>
-      <c r="R57" s="76">
+      <c r="Q57" s="68"/>
+      <c r="R57" s="26">
         <v>0.30651679018571898</v>
       </c>
-      <c r="S57" s="76">
+      <c r="S57" s="26">
         <v>0.30525380579849998</v>
       </c>
-      <c r="T57" s="79"/>
-    </row>
-    <row r="58" spans="1:20" s="85" customFormat="1" ht="19" thickBot="1">
-      <c r="A58" s="81" t="s">
+      <c r="T57" s="25"/>
+    </row>
+    <row r="58" spans="1:20" s="73" customFormat="1" ht="19" thickBot="1">
+      <c r="A58" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="81"/>
-      <c r="C58" s="82">
+      <c r="B58" s="79"/>
+      <c r="C58" s="70">
         <v>0.54746153846039702</v>
       </c>
-      <c r="D58" s="82">
+      <c r="D58" s="70">
         <v>0.53770173408211497</v>
       </c>
-      <c r="E58" s="82"/>
-      <c r="F58" s="83"/>
-      <c r="G58" s="82">
+      <c r="E58" s="70"/>
+      <c r="F58" s="71"/>
+      <c r="G58" s="70">
         <v>0.42255128327168401</v>
       </c>
-      <c r="H58" s="82">
+      <c r="H58" s="70">
         <v>0.43175680643013697</v>
       </c>
-      <c r="I58" s="82">
+      <c r="I58" s="70">
         <v>0.43747292110979902</v>
       </c>
-      <c r="J58" s="82">
+      <c r="J58" s="70">
         <v>0.43198435941931002</v>
       </c>
-      <c r="K58" s="82">
+      <c r="K58" s="70">
         <v>0.42590034085561401</v>
       </c>
-      <c r="L58" s="82">
+      <c r="L58" s="70">
         <v>0.42393576890530899</v>
       </c>
-      <c r="M58" s="82">
+      <c r="M58" s="70">
         <v>0.42589785812770797</v>
       </c>
-      <c r="N58" s="82">
+      <c r="N58" s="70">
         <v>0.42393576890530899</v>
       </c>
-      <c r="O58" s="82">
+      <c r="O58" s="70">
         <v>0.41922160182742602</v>
       </c>
-      <c r="P58" s="82">
+      <c r="P58" s="70">
         <v>0.42034096056484699</v>
       </c>
-      <c r="Q58" s="84"/>
-      <c r="R58" s="82">
+      <c r="Q58" s="72"/>
+      <c r="R58" s="70">
         <v>0.417582741528158</v>
       </c>
-      <c r="S58" s="82">
+      <c r="S58" s="70">
         <v>0.41171621609664799</v>
       </c>
-      <c r="T58" s="83"/>
+      <c r="T58" s="71"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" ht="18">
-      <c r="A59" s="69" t="s">
+      <c r="A59" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="69"/>
+      <c r="B59" s="77"/>
       <c r="C59" s="25"/>
       <c r="D59" s="26">
         <v>0.26778255025429998</v>
@@ -6273,7 +6077,7 @@
       <c r="P59" s="26">
         <v>0.178716945075508</v>
       </c>
-      <c r="Q59" s="73">
+      <c r="Q59" s="68">
         <v>0.182305931831207</v>
       </c>
       <c r="R59" s="26">
@@ -6285,10 +6089,10 @@
       <c r="T59" s="25"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" ht="18">
-      <c r="A60" s="69" t="s">
+      <c r="A60" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="69"/>
+      <c r="B60" s="77"/>
       <c r="C60" s="25"/>
       <c r="D60" s="26">
         <v>0.37533459208140602</v>
@@ -6313,7 +6117,7 @@
       <c r="P60" s="26">
         <v>0.31454773176145001</v>
       </c>
-      <c r="Q60" s="73">
+      <c r="Q60" s="68">
         <v>0.31454055609685599</v>
       </c>
       <c r="R60" s="26">
@@ -6325,10 +6129,10 @@
       <c r="T60" s="25"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" ht="18">
-      <c r="A61" s="69" t="s">
+      <c r="A61" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="69"/>
+      <c r="B61" s="77"/>
       <c r="C61" s="25"/>
       <c r="D61" s="26">
         <v>0.517477101188352</v>
@@ -6353,7 +6157,7 @@
       <c r="P61" s="26">
         <v>0.42274926975159699</v>
       </c>
-      <c r="Q61" s="71"/>
+      <c r="Q61" s="66"/>
       <c r="R61" s="26">
         <v>0.42147627414234801</v>
       </c>
@@ -6363,14 +6167,14 @@
       <c r="T61" s="25"/>
     </row>
     <row r="62" spans="1:20" ht="18">
-      <c r="N62" s="65"/>
+      <c r="N62" s="64"/>
     </row>
     <row r="63" spans="1:20">
-      <c r="A63" s="61" t="s">
+      <c r="A63" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="Q63" s="74" t="s">
-        <v>119</v>
+      <c r="Q63" s="69" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -6385,26 +6189,431 @@
     <mergeCell ref="A59:B59"/>
   </mergeCells>
   <conditionalFormatting sqref="A54 C54:XFD54">
-    <cfRule type="top10" dxfId="13" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55 C55:XFD55">
-    <cfRule type="top10" dxfId="12" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:XFD56">
+    <cfRule type="top10" dxfId="4" priority="3" stopIfTrue="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:XFD57">
+    <cfRule type="top10" dxfId="3" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:XFD59">
-    <cfRule type="top10" dxfId="11" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="5" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:XFD60">
+    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:XFD61">
-    <cfRule type="top10" dxfId="10" priority="4" stopIfTrue="1" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:XFD56">
-    <cfRule type="top10" dxfId="9" priority="3" stopIfTrue="1" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57:XFD57">
-    <cfRule type="top10" dxfId="8" priority="2" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:XFD60">
-    <cfRule type="top10" dxfId="7" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="4" stopIfTrue="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42E0D3A-D8E4-D743-8544-91C8B8E87D12}">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="31">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="32">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="35">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="35">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="35">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="29">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="34">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="31">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="35">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="29">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="33">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="33">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="29">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="28">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="28">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="92">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="28">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="34">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="32">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="35">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="31">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="34">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="31">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="32">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="35">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="32">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="29">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="31">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="32">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="32">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="33">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B44">
+    <sortCondition descending="1" ref="B1:B44"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>